<commit_message>
Updates to figure 1 labels
</commit_message>
<xml_diff>
--- a/Phenotypic Analysis/Tripsacum_greenhouse_metadata.xlsx
+++ b/Phenotypic Analysis/Tripsacum_greenhouse_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kansas-my.sharepoint.com/personal/j853s117_home_ku_edu/Documents/Wagner Postdoc/Tripsacum_Water_Stress_Anatomy/Data_analysis/Phenotypic_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kansas-my.sharepoint.com/personal/j853s117_home_ku_edu/Documents/Wagner Postdoc/Tripsacum_Water_Stress_Anatomy/GITHUB/Tripsacum-dactyloides-Root-Anatomical-Responses-to-Drought-and-Waterlogging/Phenotypic Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102" documentId="11_F35A7F04DB55FEEAA43A5378155E49121EFD4829" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F2BB38E-72E1-4787-924D-DEA5CFFC273F}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="11_F35A7F04DB55FEEAA43A5378155E49121EFD4829" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC260F50-6243-49BB-8BBB-2CAAE9C275E4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -287,18 +287,9 @@
     <t>treatment</t>
   </si>
   <si>
-    <t>Flood24</t>
-  </si>
-  <si>
-    <t>Flood72</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
-    <t>Flood48</t>
-  </si>
-  <si>
     <t>Control</t>
   </si>
   <si>
@@ -336,6 +327,15 @@
   </si>
   <si>
     <t>DAP 14</t>
+  </si>
+  <si>
+    <t>Waterlogged 24</t>
+  </si>
+  <si>
+    <t>Waterlogged 72</t>
+  </si>
+  <si>
+    <t>Waterlogged 48</t>
   </si>
 </sst>
 </file>
@@ -741,7 +741,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I86" sqref="I86"/>
+      <selection pane="topRight" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,31 +769,31 @@
         <v>81</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>96</v>
-      </c>
       <c r="J1" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -801,10 +801,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="D2" s="5">
         <v>240</v>
@@ -840,10 +840,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="D3" s="5">
         <v>136</v>
@@ -878,10 +878,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D4" s="5">
         <v>71</v>
@@ -910,10 +910,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="D5" s="5">
         <v>92</v>
@@ -948,10 +948,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D6" s="5">
         <v>182</v>
@@ -986,10 +986,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D7" s="5">
         <v>110</v>
@@ -1024,10 +1024,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D8" s="5">
         <v>246</v>
@@ -1062,10 +1062,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D9" s="5">
         <v>66</v>
@@ -1094,10 +1094,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D10" s="5">
         <v>182</v>
@@ -1132,10 +1132,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D11" s="5">
         <v>119</v>
@@ -1170,10 +1170,10 @@
         <v>12</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="D12" s="5">
         <v>236</v>
@@ -1208,10 +1208,10 @@
         <v>13</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D13" s="5">
         <v>46</v>
@@ -1240,10 +1240,10 @@
         <v>14</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D14" s="5">
         <v>131</v>
@@ -1278,10 +1278,10 @@
         <v>15</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D15" s="5">
         <v>97</v>
@@ -1310,10 +1310,10 @@
         <v>16</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="D16" s="5">
         <v>200</v>
@@ -1348,10 +1348,10 @@
         <v>17</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="D17" s="5">
         <v>100</v>
@@ -1386,10 +1386,10 @@
         <v>18</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D18" s="5">
         <v>82</v>
@@ -1418,10 +1418,10 @@
         <v>19</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="D19" s="5">
         <v>190</v>
@@ -1456,10 +1456,10 @@
         <v>20</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D20" s="5">
         <v>26</v>
@@ -1488,10 +1488,10 @@
         <v>21</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="D21" s="5">
         <v>139</v>
@@ -1526,10 +1526,10 @@
         <v>22</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D22" s="5">
         <v>126</v>
@@ -1564,10 +1564,10 @@
         <v>23</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="D23" s="5">
         <v>133</v>
@@ -1602,10 +1602,10 @@
         <v>24</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="D24" s="5">
         <v>140</v>
@@ -1640,10 +1640,10 @@
         <v>25</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="D25" s="5">
         <v>119</v>
@@ -1678,10 +1678,10 @@
         <v>26</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="D26" s="5">
         <v>126</v>
@@ -1716,10 +1716,10 @@
         <v>27</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="D27" s="5">
         <v>121</v>
@@ -1754,10 +1754,10 @@
         <v>28</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D28" s="5">
         <v>103</v>
@@ -1792,10 +1792,10 @@
         <v>29</v>
       </c>
       <c r="B29" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="D29" s="5">
         <v>186</v>
@@ -1830,10 +1830,10 @@
         <v>30</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D30" s="5">
         <v>60</v>
@@ -1862,10 +1862,10 @@
         <v>31</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="D31" s="5">
         <v>120</v>
@@ -1900,10 +1900,10 @@
         <v>32</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="D32" s="5">
         <v>117</v>
@@ -1938,10 +1938,10 @@
         <v>33</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D33" s="5">
         <v>140</v>
@@ -1976,10 +1976,10 @@
         <v>34</v>
       </c>
       <c r="B34" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="D34" s="5">
         <v>128</v>
@@ -2014,10 +2014,10 @@
         <v>35</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D35" s="5">
         <v>85</v>
@@ -2046,10 +2046,10 @@
         <v>36</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D36" s="5">
         <v>20</v>
@@ -2078,10 +2078,10 @@
         <v>37</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D37" s="5">
         <v>59</v>
@@ -2110,10 +2110,10 @@
         <v>38</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D38" s="5">
         <v>137</v>
@@ -2148,10 +2148,10 @@
         <v>39</v>
       </c>
       <c r="B39" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="D39" s="5">
         <v>102</v>
@@ -2186,10 +2186,10 @@
         <v>40</v>
       </c>
       <c r="B40" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>98</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>85</v>
       </c>
       <c r="D40" s="5">
         <v>130</v>
@@ -2224,10 +2224,10 @@
         <v>41</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="D41" s="5">
         <v>141</v>
@@ -2262,10 +2262,10 @@
         <v>42</v>
       </c>
       <c r="B42" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="D42" s="5">
         <v>196</v>
@@ -2300,10 +2300,10 @@
         <v>43</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D43" s="5">
         <v>150</v>
@@ -2338,10 +2338,10 @@
         <v>44</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="D44" s="5">
         <v>115</v>
@@ -2376,10 +2376,10 @@
         <v>45</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D45" s="5">
         <v>50</v>
@@ -2408,10 +2408,10 @@
         <v>46</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D46" s="5">
         <v>102</v>
@@ -2446,10 +2446,10 @@
         <v>47</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D47" s="5">
         <v>119</v>
@@ -2484,10 +2484,10 @@
         <v>48</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D48" s="5">
         <v>136</v>
@@ -2522,10 +2522,10 @@
         <v>49</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="D49" s="5">
         <v>189</v>
@@ -2560,10 +2560,10 @@
         <v>50</v>
       </c>
       <c r="B50" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C50" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="D50" s="5">
         <v>100</v>
@@ -2598,10 +2598,10 @@
         <v>51</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D51" s="5">
         <v>164</v>
@@ -2636,10 +2636,10 @@
         <v>52</v>
       </c>
       <c r="B52" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C52" s="5" t="s">
         <v>98</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>85</v>
       </c>
       <c r="D52" s="5">
         <v>160</v>
@@ -2674,10 +2674,10 @@
         <v>53</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D53" s="5">
         <v>76</v>
@@ -2706,10 +2706,10 @@
         <v>54</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D54" s="5">
         <v>148</v>
@@ -2744,10 +2744,10 @@
         <v>55</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D55" s="5">
         <v>185</v>
@@ -2782,10 +2782,10 @@
         <v>56</v>
       </c>
       <c r="B56" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="D56" s="5">
         <v>127</v>
@@ -2820,10 +2820,10 @@
         <v>57</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="D57" s="5">
         <v>135</v>
@@ -2858,10 +2858,10 @@
         <v>58</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="D58" s="5">
         <v>149</v>
@@ -2896,10 +2896,10 @@
         <v>59</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="D59" s="5">
         <v>140</v>
@@ -2934,10 +2934,10 @@
         <v>60</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D60" s="5">
         <v>9</v>
@@ -2966,10 +2966,10 @@
         <v>61</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D61" s="5">
         <v>58</v>
@@ -2998,10 +2998,10 @@
         <v>62</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="D62" s="5">
         <v>85</v>
@@ -3036,10 +3036,10 @@
         <v>63</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D63" s="5">
         <v>156</v>
@@ -3074,10 +3074,10 @@
         <v>64</v>
       </c>
       <c r="B64" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C64" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="D64" s="5">
         <v>267</v>
@@ -3112,10 +3112,10 @@
         <v>65</v>
       </c>
       <c r="B65" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C65" s="5" t="s">
         <v>98</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>85</v>
       </c>
       <c r="D65" s="5">
         <v>116</v>
@@ -3150,10 +3150,10 @@
         <v>66</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D66" s="5">
         <v>83</v>
@@ -3182,10 +3182,10 @@
         <v>67</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D67" s="5">
         <v>115</v>
@@ -3220,10 +3220,10 @@
         <v>68</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D68" s="5">
         <v>124</v>
@@ -3258,10 +3258,10 @@
         <v>69</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D69" s="5">
         <v>121</v>
@@ -3296,10 +3296,10 @@
         <v>70</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D70" s="5">
         <v>19</v>
@@ -3328,10 +3328,10 @@
         <v>71</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="D71" s="5">
         <v>235</v>
@@ -3366,10 +3366,10 @@
         <v>72</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D72" s="5">
         <v>290</v>
@@ -3404,10 +3404,10 @@
         <v>73</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="D73" s="5">
         <v>123</v>
@@ -3442,10 +3442,10 @@
         <v>74</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="D74" s="5">
         <v>128</v>
@@ -3480,10 +3480,10 @@
         <v>75</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D75" s="5">
         <v>205</v>
@@ -3518,10 +3518,10 @@
         <v>76</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D76" s="5">
         <v>129</v>
@@ -3556,10 +3556,10 @@
         <v>77</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D77" s="5">
         <v>74</v>
@@ -3588,10 +3588,10 @@
         <v>78</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D78" s="5">
         <v>50</v>
@@ -3620,10 +3620,10 @@
         <v>79</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="D79" s="5">
         <v>180</v>
@@ -3658,10 +3658,10 @@
         <v>80</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D80" s="5">
         <v>65</v>

</xml_diff>